<commit_message>
Add framwork/test cases with color and New Spreadsheets
</commit_message>
<xml_diff>
--- a/src/test/resources/etalon/comparetwosheets/CTS_005_duplicatesFillWithColor.xlsx
+++ b/src/test/resources/etalon/comparetwosheets/CTS_005_duplicatesFillWithColor.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="189" yWindow="583" windowWidth="32537" windowHeight="14409"/>
   </bookViews>
   <sheets>
-    <sheet name="Result" sheetId="3" r:id="rId1"/>
+    <sheet name="Table1" sheetId="3" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -369,7 +369,7 @@
   <dimension ref="C1:I1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>